<commit_message>
course end date update
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Madarsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FBBFD80-FF7C-4FAB-898D-807F66AB9880}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EA301DE-2DFF-44DC-ADAB-5FD4BDECB39F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2055" yWindow="1065" windowWidth="16215" windowHeight="9615" xr2:uid="{9269FCFB-9384-4701-B347-1BC29F823C38}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9269FCFB-9384-4701-B347-1BC29F823C38}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="29">
   <si>
     <t>id</t>
   </si>
@@ -100,9 +100,6 @@
     <t>(F),(I)</t>
   </si>
   <si>
-    <t>teacher</t>
-  </si>
-  <si>
     <t>teach_id</t>
   </si>
   <si>
@@ -128,6 +125,27 @@
   </si>
   <si>
     <t>Hpl_id</t>
+  </si>
+  <si>
+    <t>Teacher</t>
+  </si>
+  <si>
+    <t>att_id</t>
+  </si>
+  <si>
+    <t>att_pass</t>
+  </si>
+  <si>
+    <t>Attendance_header</t>
+  </si>
+  <si>
+    <t>Attendance_details</t>
+  </si>
+  <si>
+    <t>att_status</t>
+  </si>
+  <si>
+    <t>year</t>
   </si>
 </sst>
 </file>
@@ -501,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44B3E671-55BA-4822-9AC9-1302385AB835}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,18 +530,21 @@
     <col min="1" max="1" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -531,24 +552,30 @@
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
       </c>
       <c r="I2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I3" t="s">
         <v>7</v>
@@ -556,8 +583,14 @@
       <c r="J3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -565,13 +598,16 @@
         <v>12</v>
       </c>
       <c r="I4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -581,40 +617,49 @@
       <c r="I5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="I6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E8" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" t="s">
-        <v>14</v>
       </c>
       <c r="F8" t="s">
         <v>11</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
       <c r="E9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I9" t="s">
         <v>0</v>
@@ -622,35 +667,53 @@
       <c r="J9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L9" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L10" t="s">
+        <v>23</v>
+      </c>
+      <c r="M10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
       <c r="I11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J11" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L11" t="s">
+        <v>19</v>
+      </c>
+      <c r="M11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -658,7 +721,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>8</v>
       </c>

</xml_diff>